<commit_message>
cleaning the previous code with more generic implementations
</commit_message>
<xml_diff>
--- a/src/test/resources/output/Annotated.xlsx
+++ b/src/test/resources/output/Annotated.xlsx
@@ -123,7 +123,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Generated on: Tue Mar 10 00:59:15 IST 2020</t>
+          <t>Generated on: Fri Mar 26 23:51:27 WEST 2021</t>
         </is>
       </c>
     </row>
@@ -194,11 +194,9 @@
         <v>43899.958645833336</v>
       </c>
       <c r="G5" s="7" t="n">
-        <v>33026.88402777778</v>
-      </c>
-      <c r="H5" s="8" t="n">
-        <v>0.124</v>
-      </c>
+        <v>33026.48819444444</v>
+      </c>
+      <c r="H5"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -222,11 +220,9 @@
         <v>43899.958645833336</v>
       </c>
       <c r="G6" s="7" t="n">
-        <v>42048.10555555556</v>
-      </c>
-      <c r="H6" s="8" t="n">
-        <v>1.0</v>
-      </c>
+        <v>42047.66805555556</v>
+      </c>
+      <c r="H6"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:H4"/>

</xml_diff>